<commit_message>
Updated forms and UI fixes
</commit_message>
<xml_diff>
--- a/config/forms/app/case_contact_follow_up.xlsx
+++ b/config/forms/app/case_contact_follow_up.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\morlig\icap\dmi-adam-zwei\config\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\morlig\icap\dmi-adam\config\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B8960C-737B-437B-96B7-BCB486D79269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D8E85B-3A87-48FB-B9BA-F19599A7DED5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{06C34439-B795-40B6-B34E-E6B3C4A90C1D}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="107">
   <si>
     <t>form_title</t>
   </si>
@@ -298,9 +298,6 @@
     <t>case_contact_follow_up</t>
   </si>
   <si>
-    <t>case_name</t>
-  </si>
-  <si>
     <t>case_contact_name</t>
   </si>
   <si>
@@ -319,43 +316,49 @@
     <t>integer</t>
   </si>
   <si>
-    <t>outbreak_name</t>
-  </si>
-  <si>
     <t>../inputs/contact/parent/parent/name</t>
   </si>
   <si>
-    <t>case_number</t>
-  </si>
-  <si>
-    <t>../inputs/contact/parent/_id</t>
-  </si>
-  <si>
-    <t>outbreak_code</t>
-  </si>
-  <si>
     <t>../inputs/contact/parent/parent/code</t>
   </si>
   <si>
     <t>note</t>
   </si>
   <si>
-    <t>case_number_title</t>
-  </si>
-  <si>
-    <t>case_title</t>
-  </si>
-  <si>
-    <t>&lt;h4 style="padding: 5px 0;"&gt;Case Number: ${case_number} &lt;/h4&gt;</t>
-  </si>
-  <si>
     <t>case_identifier_title</t>
   </si>
   <si>
     <t>&lt;h3 style="border-bottom: #f47b63 solid 2px; padding: 5px 0;"&gt;Signs &amp; Symptoms&lt;/h3&gt;</t>
   </si>
   <si>
-    <t>&lt;h4 style="padding: 5px 0;"&gt;${outbreak_name} &gt; ${case_name} &gt; ${case_contact_name} &lt;/h4&gt;</t>
+    <t>patient_id</t>
+  </si>
+  <si>
+    <t>../inputs/contact/parent/patient_id</t>
+  </si>
+  <si>
+    <t>case_id_title</t>
+  </si>
+  <si>
+    <t>case_name_title</t>
+  </si>
+  <si>
+    <t>cfu_case_id</t>
+  </si>
+  <si>
+    <t>cfu_case_name</t>
+  </si>
+  <si>
+    <t>cfu_outbreak_code</t>
+  </si>
+  <si>
+    <t>cfu_outbreak_name</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="padding: 5px 0;"&gt;${cfu_outbreak_name} &gt; ${cfu_case_name} &gt; ${case_contact_name} &lt;/h4&gt;</t>
+  </si>
+  <si>
+    <t>&lt;h4 style="padding: 5px 0;"&gt;Case ID: ${cfu_case_id} &lt;/h4&gt;</t>
   </si>
 </sst>
 </file>
@@ -866,12 +869,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6DDD78E-1CAD-40FF-A32D-5B3923D727A1}">
-  <dimension ref="A1:P50"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1229,7 +1232,7 @@
         <v>34</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>32</v>
@@ -1249,9 +1252,15 @@
       <c r="P19" s="7"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
+      <c r="A20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>32</v>
+      </c>
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1266,47 +1275,41 @@
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
     </row>
-    <row r="21" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="17" t="s">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+    </row>
+    <row r="22" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="7"/>
-      <c r="K22" s="7"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="7"/>
-      <c r="N22" s="7"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="7"/>
+      <c r="C22" s="17" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>34</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>32</v>
@@ -1330,7 +1333,7 @@
         <v>34</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>73</v>
+        <v>9</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>32</v>
@@ -1349,13 +1352,29 @@
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
     </row>
-    <row r="25" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="17" t="s">
-        <v>40</v>
-      </c>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
     </row>
     <row r="26" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="17" t="s">
@@ -1370,7 +1389,7 @@
         <v>41</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.35">
@@ -1378,41 +1397,23 @@
         <v>41</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" s="17" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C30" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13"/>
-      <c r="H30" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I30" s="13"/>
-      <c r="J30" s="13"/>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="M30" s="13"/>
-      <c r="N30" s="13"/>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
     </row>
     <row r="31" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>87</v>
+        <v>45</v>
       </c>
       <c r="C31" s="14" t="s">
         <v>32</v>
@@ -1422,7 +1423,7 @@
       <c r="F31" s="13"/>
       <c r="G31" s="13"/>
       <c r="H31" s="13" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="13"/>
@@ -1433,12 +1434,12 @@
       <c r="O31" s="13"/>
       <c r="P31" s="13"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="13" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>32</v>
@@ -1448,7 +1449,7 @@
       <c r="F32" s="13"/>
       <c r="G32" s="13"/>
       <c r="H32" s="13" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
@@ -1464,7 +1465,7 @@
         <v>43</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="C33" s="14" t="s">
         <v>32</v>
@@ -1474,7 +1475,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="13"/>
       <c r="H33" s="13" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="I33" s="13"/>
       <c r="J33" s="13"/>
@@ -1490,7 +1491,7 @@
         <v>43</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>32</v>
@@ -1500,7 +1501,7 @@
       <c r="F34" s="13"/>
       <c r="G34" s="13"/>
       <c r="H34" s="13" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="13"/>
@@ -1516,7 +1517,7 @@
         <v>43</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>32</v>
@@ -1526,7 +1527,7 @@
       <c r="F35" s="13"/>
       <c r="G35" s="13"/>
       <c r="H35" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I35" s="13"/>
       <c r="J35" s="13"/>
@@ -1537,115 +1538,127 @@
       <c r="O35" s="13"/>
       <c r="P35" s="13"/>
     </row>
-    <row r="37" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="9" t="s">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="13"/>
+      <c r="M36" s="13"/>
+      <c r="N36" s="13"/>
+      <c r="O36" s="13"/>
+      <c r="P36" s="13"/>
+    </row>
+    <row r="38" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B38" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I37" s="9" t="s">
+      <c r="C38" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I38" s="9" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="B40" s="18" t="s">
-        <v>103</v>
-      </c>
       <c r="C40" s="18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" t="s">
-        <v>88</v>
-      </c>
-      <c r="C42" t="s">
-        <v>89</v>
-      </c>
-      <c r="E42" t="s">
-        <v>12</v>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" s="18" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B43" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E43" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="10" t="s">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B45" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="46" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9" t="s">
+    <row r="47" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="B46" s="12" t="s">
+      <c r="B47" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="I46" s="9" t="s">
+      <c r="C47" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="I47" s="9" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="C47" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -1653,13 +1666,13 @@
         <v>43</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="49" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
@@ -1667,20 +1680,34 @@
         <v>43</v>
       </c>
       <c r="B49" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H49" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="16" t="s">
         <v>81</v>
       </c>
-      <c r="C49" s="16" t="s">
+      <c r="C50" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="H49" s="16" t="s">
+      <c r="H50" s="16" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A50" s="10" t="s">
+    <row r="51" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="B51" s="10" t="s">
         <v>74</v>
       </c>
     </row>

</xml_diff>